<commit_message>
change for the new method, change name
</commit_message>
<xml_diff>
--- a/data/hicp_all.xlsx
+++ b/data/hicp_all.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lananhnguyen/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lananhnguyen/Desktop/thesis/thesis_code/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96447BD6-7BE3-B54D-88A2-823DFCED4CA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA5B0B0-25F7-784E-A3FC-A21073AB3A7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4484,7 +4484,7 @@
       <pane xSplit="1" ySplit="10" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A9" sqref="A9:XFD11"/>
+      <selection pane="bottomRight" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>